<commit_message>
Update biofuels, calibration, heat generation
</commit_message>
<xml_diff>
--- a/TEMOA_Europe_Results/Elastic demand.xlsx
+++ b/TEMOA_Europe_Results/Elastic demand.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D7D55017-2FAD-440C-BAA5-0F239D20C269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C11E6E4-A9D8-4968-AB6D-A8AE7F7626BB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D7D55017-2FAD-440C-BAA5-0F239D20C269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE00857-0FAE-47DE-9391-8EC7723C3CDF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paper" sheetId="4" r:id="rId1"/>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -187,6 +187,15 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -363,31 +372,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-2.2457682046742198</c:v>
+                  <c:v>9.0316922644172806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.280834485778101</c:v>
+                  <c:v>8.9898262698002593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.535048440452002</c:v>
+                  <c:v>15.0232392376651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.293468341928197</c:v>
+                  <c:v>34.711977233204898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.211540691266102</c:v>
+                  <c:v>21.1760512654979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.977247037745601</c:v>
+                  <c:v>4.1497894416852104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2088787852442899</c:v>
+                  <c:v>-5.1040443793511603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.4651798005117804</c:v>
+                  <c:v>-122.652753393711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.3714064045683703</c:v>
+                  <c:v>-66.369555750769905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1189,13 +1198,13 @@
                   <c:v>104.08924346358154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.2763784786966</c:v>
+                  <c:v>91.539120647426685</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.92055085792178</c:v>
+                  <c:v>100.1672781943241</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111.40803418055052</c:v>
+                  <c:v>111.02026821518092</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>115.89259929947073</c:v>
@@ -1360,7 +1369,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
-          <c:min val="100"/>
+          <c:min val="80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1748,13 +1757,13 @@
                   <c:v>104.08924346358154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.2763784786966</c:v>
+                  <c:v>91.539120647426685</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.92055085792178</c:v>
+                  <c:v>100.1672781943241</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111.40803418055052</c:v>
+                  <c:v>111.02026821518092</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>115.89259929947073</c:v>
@@ -2244,31 +2253,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-2.2457682046742198</c:v>
+                  <c:v>9.0316922644172806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.280834485778101</c:v>
+                  <c:v>8.9898262698002593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.535048440452002</c:v>
+                  <c:v>15.0232392376651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.293468341928197</c:v>
+                  <c:v>34.711977233204898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.211540691266102</c:v>
+                  <c:v>21.1760512654979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.977247037745601</c:v>
+                  <c:v>4.1497894416852104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2088787852442899</c:v>
+                  <c:v>-5.1040443793511603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.4651798005117804</c:v>
+                  <c:v>-122.652753393711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.3714064045683703</c:v>
+                  <c:v>-66.369555750769905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2973,13 +2982,13 @@
                   <c:v>218.08170670197262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>218.72522005317757</c:v>
+                  <c:v>174.92478288153185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>239.97339950243591</c:v>
+                  <c:v>204.59498957328589</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>243.24930849017187</c:v>
+                  <c:v>241.91587243757215</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>247.18545108624559</c:v>
@@ -3469,31 +3478,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-2.2457682046742198</c:v>
+                  <c:v>9.0316922644172806</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.280834485778101</c:v>
+                  <c:v>8.9898262698002593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.535048440452002</c:v>
+                  <c:v>15.0232392376651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.293468341928197</c:v>
+                  <c:v>34.711977233204898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.211540691266102</c:v>
+                  <c:v>21.1760512654979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.977247037745601</c:v>
+                  <c:v>4.1497894416852104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2088787852442899</c:v>
+                  <c:v>-5.1040443793511603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.4651798005117804</c:v>
+                  <c:v>-122.652753393711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.3714064045683703</c:v>
+                  <c:v>-66.369555750769905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4228,13 +4237,13 @@
                   <c:v>521.36736106537296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>522.64090880675337</c:v>
+                  <c:v>435.95747368147954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>564.93223294325207</c:v>
+                  <c:v>494.67641812578427</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>571.17540677771956</c:v>
+                  <c:v>568.53646467980707</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>580.48859472124275</c:v>
@@ -4595,7 +4604,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.17534492563429571"/>
           <c:y val="0.17171296296296298"/>
-          <c:w val="0.79965507436570427"/>
+          <c:w val="0.53568756235450621"/>
           <c:h val="0.51681284631087776"/>
         </c:manualLayout>
       </c:layout>
@@ -4786,13 +4795,13 @@
                   <c:v>521.36736106537296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>522.64090880675337</c:v>
+                  <c:v>435.95747368147954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>564.93223294325207</c:v>
+                  <c:v>494.67641812578427</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>571.17540677771956</c:v>
+                  <c:v>568.53646467980707</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>580.48859472124275</c:v>
@@ -5214,13 +5223,13 @@
                   <c:v>218.08170670197262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>218.72522005317757</c:v>
+                  <c:v>174.92478288153185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>239.97339950243591</c:v>
+                  <c:v>204.59498957328589</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>243.24930849017187</c:v>
+                  <c:v>241.91587243757215</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>247.18545108624559</c:v>
@@ -5369,7 +5378,7 @@
         <c:axId val="363981039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="200"/>
+          <c:min val="160"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5489,7 +5498,7 @@
         <c:crossAx val="462803391"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="20"/>
+        <c:majorUnit val="40"/>
         <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
@@ -5806,13 +5815,13 @@
                   <c:v>521.36736106537296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>522.64090880675337</c:v>
+                  <c:v>435.95747368147954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>564.93223294325207</c:v>
+                  <c:v>494.67641812578427</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>571.17540677771956</c:v>
+                  <c:v>568.53646467980707</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>580.48859472124275</c:v>
@@ -5976,8 +5985,8 @@
         <c:axId val="363981039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="620"/>
-          <c:min val="500"/>
+          <c:max val="660"/>
+          <c:min val="420"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6040,7 +6049,7 @@
         <c:crossAx val="462803391"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="40"/>
+        <c:majorUnit val="80"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
@@ -12454,8 +12463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D021FE-ACF9-495C-B830-1D7A4EA0C94C}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12509,8 +12518,8 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E2" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -12521,7 +12530,7 @@
       </c>
       <c r="K2" s="13">
         <f>E2</f>
-        <v>-2.2457682046742198</v>
+        <v>9.0316922644172806</v>
       </c>
       <c r="L2" s="13">
         <f>F2</f>
@@ -12544,8 +12553,8 @@
       <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E3" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -12556,7 +12565,7 @@
       </c>
       <c r="K3" s="13">
         <f>E11</f>
-        <v>24.280834485778101</v>
+        <v>8.9898262698002593</v>
       </c>
       <c r="L3" s="13">
         <f>F11</f>
@@ -12580,8 +12589,8 @@
       <c r="D4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E4" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -12592,7 +12601,7 @@
       </c>
       <c r="K4" s="13">
         <f>E20</f>
-        <v>63.535048440452002</v>
+        <v>15.0232392376651</v>
       </c>
       <c r="L4" s="13">
         <f>F20</f>
@@ -12615,8 +12624,8 @@
       <c r="D5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E5" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -12627,7 +12636,7 @@
       </c>
       <c r="K5" s="13">
         <f>E29</f>
-        <v>62.293468341928197</v>
+        <v>34.711977233204898</v>
       </c>
       <c r="L5" s="13">
         <f>F29</f>
@@ -12650,8 +12659,8 @@
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E6" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -12662,7 +12671,7 @@
       </c>
       <c r="K6" s="13">
         <f>E38</f>
-        <v>18.211540691266102</v>
+        <v>21.1760512654979</v>
       </c>
       <c r="L6" s="13">
         <f>F38</f>
@@ -12685,8 +12694,8 @@
       <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E7" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -12697,7 +12706,7 @@
       </c>
       <c r="K7" s="13">
         <f>E47</f>
-        <v>14.977247037745601</v>
+        <v>4.1497894416852104</v>
       </c>
       <c r="L7" s="13">
         <f>F47</f>
@@ -12720,8 +12729,8 @@
       <c r="D8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E8" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -12732,7 +12741,7 @@
       </c>
       <c r="K8" s="13">
         <f>E56</f>
-        <v>-1.2088787852442899</v>
+        <v>-5.1040443793511603</v>
       </c>
       <c r="L8" s="13">
         <f>F56</f>
@@ -12755,8 +12764,8 @@
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E9" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -12767,7 +12776,7 @@
       </c>
       <c r="K9" s="13">
         <f>E66</f>
-        <v>-4.4651798005117804</v>
+        <v>-122.652753393711</v>
       </c>
       <c r="L9" s="13">
         <f>F66</f>
@@ -12790,8 +12799,8 @@
       <c r="D10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E10" s="17">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -12802,7 +12811,7 @@
       </c>
       <c r="K10" s="13">
         <f>E74</f>
-        <v>-6.3714064045683703</v>
+        <v>-66.369555750769905</v>
       </c>
       <c r="L10" s="13">
         <f>F74</f>
@@ -12825,8 +12834,8 @@
       <c r="D11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="9">
-        <v>24.280834485778101</v>
+      <c r="E11" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -12844,8 +12853,8 @@
       <c r="D12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="9">
-        <v>24.280834485778101</v>
+      <c r="E12" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -12868,8 +12877,8 @@
       <c r="D13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="9">
-        <v>24.280834485778101</v>
+      <c r="E13" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -12892,8 +12901,8 @@
       <c r="D14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="9">
-        <v>24.280834485778101</v>
+      <c r="E14" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -12910,8 +12919,8 @@
       <c r="D15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="9">
-        <v>24.280834485778101</v>
+      <c r="E15" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -12934,8 +12943,8 @@
       <c r="D16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="9">
-        <v>24.280834485778101</v>
+      <c r="E16" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -12963,8 +12972,8 @@
       <c r="D17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="9">
-        <v>24.280834485778101</v>
+      <c r="E17" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -12996,8 +13005,8 @@
       <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="9">
-        <v>24.280834485778101</v>
+      <c r="E18" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -13034,8 +13043,8 @@
       <c r="D19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="9">
-        <v>24.280834485778101</v>
+      <c r="E19" s="17">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -13071,8 +13080,8 @@
       <c r="D20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="9">
-        <v>63.535048440452002</v>
+      <c r="E20" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -13108,8 +13117,8 @@
       <c r="D21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="9">
-        <v>63.535048440452002</v>
+      <c r="E21" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -13129,7 +13138,7 @@
       </c>
       <c r="M21" s="13">
         <f>IF($L$20+$K$12*$L$20/K$4*(K5-K$4)&lt;$L21,$L$20+$K$12*$L$20/K$4*(K5-K$4),$L21)</f>
-        <v>104.2763784786966</v>
+        <v>91.539120647426685</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -13145,8 +13154,8 @@
       <c r="D22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="9">
-        <v>63.535048440452002</v>
+      <c r="E22" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -13166,7 +13175,7 @@
       </c>
       <c r="M22" s="13">
         <f t="shared" ref="M22:M23" si="1">IF($L$20+$K$12*$L$20/K$4*(K6-K$4)&lt;$L22,$L$20+$K$12*$L$20/K$4*(K6-K$4),$L22)</f>
-        <v>110.92055085792178</v>
+        <v>100.1672781943241</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
@@ -13182,8 +13191,8 @@
       <c r="D23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="9">
-        <v>63.535048440452002</v>
+      <c r="E23" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -13203,7 +13212,7 @@
       </c>
       <c r="M23" s="13">
         <f t="shared" si="1"/>
-        <v>111.40803418055052</v>
+        <v>111.02026821518092</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
@@ -13219,8 +13228,8 @@
       <c r="D24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="9">
-        <v>63.535048440452002</v>
+      <c r="E24" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -13256,8 +13265,8 @@
       <c r="D25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9">
-        <v>63.535048440452002</v>
+      <c r="E25" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -13293,8 +13302,8 @@
       <c r="D26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="9">
-        <v>63.535048440452002</v>
+      <c r="E26" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -13330,8 +13339,8 @@
       <c r="D27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="9">
-        <v>63.535048440452002</v>
+      <c r="E27" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -13347,8 +13356,8 @@
       <c r="D28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="9">
-        <v>63.535048440452002</v>
+      <c r="E28" s="17">
+        <v>15.0232392376651</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -13357,8 +13366,8 @@
         <v>2025</v>
       </c>
       <c r="M28" s="16">
-        <f>M21/L21-1</f>
-        <v>-6.2106994431025075E-2</v>
+        <f t="shared" ref="M28:M33" si="3">M21/L21-1</f>
+        <v>-0.17666970944243376</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.35">
@@ -13371,8 +13380,8 @@
       <c r="D29" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="9">
-        <v>62.293468341928197</v>
+      <c r="E29" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -13381,8 +13390,8 @@
         <v>2030</v>
       </c>
       <c r="M29" s="16">
-        <f>M22/L22-1</f>
-        <v>-1.6546906537335704E-2</v>
+        <f t="shared" si="3"/>
+        <v>-0.11188847475050312</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
@@ -13395,8 +13404,8 @@
       <c r="D30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="9">
-        <v>62.293468341928197</v>
+      <c r="E30" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -13405,8 +13414,8 @@
         <v>2035</v>
       </c>
       <c r="M30" s="16">
-        <f>M23/L23-1</f>
-        <v>-2.763924459395517E-2</v>
+        <f t="shared" si="3"/>
+        <v>-3.102363612173753E-2</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.35">
@@ -13419,8 +13428,8 @@
       <c r="D31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="9">
-        <v>62.293468341928303</v>
+      <c r="E31" s="17">
+        <v>34.711977233205502</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -13431,7 +13440,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="M31" s="16">
-        <f>M24/L24-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13445,8 +13454,8 @@
       <c r="D32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="9">
-        <v>62.293468341928197</v>
+      <c r="E32" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -13455,7 +13464,7 @@
         <v>2045</v>
       </c>
       <c r="M32" s="16">
-        <f>M25/L25-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13469,8 +13478,8 @@
       <c r="D33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="9">
-        <v>62.293468341928197</v>
+      <c r="E33" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -13479,7 +13488,7 @@
         <v>2050</v>
       </c>
       <c r="M33" s="16">
-        <f>M26/L26-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13493,8 +13502,8 @@
       <c r="D34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9">
-        <v>62.293468341928303</v>
+      <c r="E34" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -13511,8 +13520,8 @@
       <c r="D35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="9">
-        <v>62.293468341928303</v>
+      <c r="E35" s="17">
+        <v>34.711977233205502</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -13529,8 +13538,8 @@
       <c r="D36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="9">
-        <v>62.293468341928303</v>
+      <c r="E36" s="17">
+        <v>34.711977233204898</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -13547,8 +13556,8 @@
       <c r="D37" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="9">
-        <v>62.293468341928197</v>
+      <c r="E37" s="17">
+        <v>34.711977233205502</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -13565,8 +13574,8 @@
       <c r="D38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="9">
-        <v>18.211540691266102</v>
+      <c r="E38" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -13583,8 +13592,8 @@
       <c r="D39" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="9">
-        <v>18.211540691266102</v>
+      <c r="E39" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -13601,8 +13610,8 @@
       <c r="D40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="9">
-        <v>18.211540691266102</v>
+      <c r="E40" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -13619,8 +13628,8 @@
       <c r="D41" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="9">
-        <v>18.211540691266102</v>
+      <c r="E41" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -13637,8 +13646,8 @@
       <c r="D42" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="9">
-        <v>18.211540691266102</v>
+      <c r="E42" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -13655,8 +13664,8 @@
       <c r="D43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="9">
-        <v>18.211540691266102</v>
+      <c r="E43" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -13673,8 +13682,8 @@
       <c r="D44" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="9">
-        <v>18.211540691266102</v>
+      <c r="E44" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -13691,8 +13700,8 @@
       <c r="D45" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="9">
-        <v>18.211540691266102</v>
+      <c r="E45" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -13709,8 +13718,8 @@
       <c r="D46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="9">
-        <v>18.211540691266102</v>
+      <c r="E46" s="17">
+        <v>21.1760512654979</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -13728,8 +13737,8 @@
       <c r="D47" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="9">
-        <v>14.977247037745601</v>
+      <c r="E47" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -13747,8 +13756,8 @@
       <c r="D48" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="9">
-        <v>14.977247037745601</v>
+      <c r="E48" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -13766,8 +13775,8 @@
       <c r="D49" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="9">
-        <v>14.977247037745601</v>
+      <c r="E49" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
@@ -13785,8 +13794,8 @@
       <c r="D50" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="9">
-        <v>14.977247037745601</v>
+      <c r="E50" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
@@ -13804,8 +13813,8 @@
       <c r="D51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="9">
-        <v>14.977247037745601</v>
+      <c r="E51" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -13823,8 +13832,8 @@
       <c r="D52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="9">
-        <v>14.977247037745601</v>
+      <c r="E52" s="17">
+        <v>4.1497894416869299</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -13842,8 +13851,8 @@
       <c r="D53" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="9">
-        <v>14.977247037745601</v>
+      <c r="E53" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -13861,8 +13870,8 @@
       <c r="D54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="9">
-        <v>14.977247037745601</v>
+      <c r="E54" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -13880,8 +13889,8 @@
       <c r="D55" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="9">
-        <v>14.977247037745601</v>
+      <c r="E55" s="17">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -13899,8 +13908,8 @@
       <c r="D56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E56" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -13918,8 +13927,8 @@
       <c r="D57" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E57" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -13937,8 +13946,8 @@
       <c r="D58" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E58" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -13956,8 +13965,8 @@
       <c r="D59" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E59" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -13975,8 +13984,8 @@
       <c r="D60" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E60" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -13994,8 +14003,8 @@
       <c r="D61" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E61" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -14013,8 +14022,8 @@
       <c r="D62" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E62" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
@@ -14032,8 +14041,8 @@
       <c r="D63" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E63" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
@@ -14050,8 +14059,8 @@
       <c r="D64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E64" s="17">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
@@ -14068,8 +14077,8 @@
       <c r="D65" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E65" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
@@ -14086,8 +14095,8 @@
       <c r="D66" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E66" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -14104,8 +14113,8 @@
       <c r="D67" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E67" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
@@ -14122,8 +14131,8 @@
       <c r="D68" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E68" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
@@ -14140,8 +14149,8 @@
       <c r="D69" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E69" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
@@ -14158,8 +14167,8 @@
       <c r="D70" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E70" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E70" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -14176,8 +14185,8 @@
       <c r="D71" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E71" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
@@ -14194,8 +14203,8 @@
       <c r="D72" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E72" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -14212,8 +14221,8 @@
       <c r="D73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E73" s="17">
+        <v>-122.652753393711</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -14230,8 +14239,8 @@
       <c r="D74" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E74" s="17">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
@@ -14248,8 +14257,8 @@
       <c r="D75" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E75" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E75" s="17">
+        <v>-56.503754088162601</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
@@ -14266,8 +14275,8 @@
       <c r="D76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E76" s="17">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
@@ -14284,8 +14293,8 @@
       <c r="D77" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E77" s="17">
+        <v>-64.375129649066494</v>
       </c>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -14302,8 +14311,8 @@
       <c r="D78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E78" s="17">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -14320,8 +14329,8 @@
       <c r="D79" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E79" s="17">
+        <v>-57.3946104489983</v>
       </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -14338,8 +14347,8 @@
       <c r="D80" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E80" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E80" s="17">
+        <v>-66.462617756164704</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
@@ -14356,8 +14365,8 @@
       <c r="D81" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E81" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E81" s="17">
+        <v>-65.583419989923399</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
@@ -14374,8 +14383,8 @@
       <c r="D82" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E82" s="17">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
@@ -14398,8 +14407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3942F0AE-02BA-46F1-82D8-C6979DFE091D}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:M33"/>
+    <sheetView topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14450,8 +14459,8 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E2" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -14465,7 +14474,7 @@
       </c>
       <c r="K2" s="13">
         <f>E2</f>
-        <v>-2.2457682046742198</v>
+        <v>9.0316922644172806</v>
       </c>
       <c r="L2" s="13">
         <f>F2</f>
@@ -14485,8 +14494,8 @@
       <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E3" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -14500,7 +14509,7 @@
       </c>
       <c r="K3" s="13">
         <f>E11</f>
-        <v>24.280834485778101</v>
+        <v>8.9898262698002593</v>
       </c>
       <c r="L3" s="13">
         <f>F11</f>
@@ -14521,8 +14530,8 @@
       <c r="D4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E4" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -14536,7 +14545,7 @@
       </c>
       <c r="K4" s="13">
         <f>E20</f>
-        <v>63.535048440452002</v>
+        <v>15.0232392376651</v>
       </c>
       <c r="L4" s="13">
         <f>F20</f>
@@ -14556,8 +14565,8 @@
       <c r="D5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E5" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -14571,7 +14580,7 @@
       </c>
       <c r="K5" s="13">
         <f>E29</f>
-        <v>62.293468341928197</v>
+        <v>34.711977233204898</v>
       </c>
       <c r="L5" s="13">
         <f>F29</f>
@@ -14591,8 +14600,8 @@
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E6" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -14606,7 +14615,7 @@
       </c>
       <c r="K6" s="13">
         <f>E38</f>
-        <v>18.211540691266102</v>
+        <v>21.1760512654979</v>
       </c>
       <c r="L6" s="13">
         <f>F38</f>
@@ -14626,8 +14635,8 @@
       <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E7" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -14641,7 +14650,7 @@
       </c>
       <c r="K7" s="13">
         <f>E47</f>
-        <v>14.977247037745601</v>
+        <v>4.1497894416852104</v>
       </c>
       <c r="L7" s="13">
         <f>F47</f>
@@ -14661,8 +14670,8 @@
       <c r="D8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E8" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -14676,7 +14685,7 @@
       </c>
       <c r="K8" s="13">
         <f>E56</f>
-        <v>-1.2088787852442899</v>
+        <v>-5.1040443793511603</v>
       </c>
       <c r="L8" s="13">
         <f>F56</f>
@@ -14696,8 +14705,8 @@
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E9" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -14711,7 +14720,7 @@
       </c>
       <c r="K9" s="13">
         <f>E66</f>
-        <v>-4.4651798005117804</v>
+        <v>-122.652753393711</v>
       </c>
       <c r="L9" s="13">
         <f>F66</f>
@@ -14731,8 +14740,8 @@
       <c r="D10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E10" s="18">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -14746,7 +14755,7 @@
       </c>
       <c r="K10" s="13">
         <f>E74</f>
-        <v>-6.3714064045683703</v>
+        <v>-66.369555750769905</v>
       </c>
       <c r="L10" s="13">
         <f>F74</f>
@@ -14766,8 +14775,8 @@
       <c r="D11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="9">
-        <v>24.280834485778101</v>
+      <c r="E11" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -14788,8 +14797,8 @@
       <c r="D12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="9">
-        <v>24.280834485778101</v>
+      <c r="E12" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -14815,8 +14824,8 @@
       <c r="D13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="9">
-        <v>24.280834485778101</v>
+      <c r="E13" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -14842,8 +14851,8 @@
       <c r="D14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="9">
-        <v>24.280834485778101</v>
+      <c r="E14" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -14863,8 +14872,8 @@
       <c r="D15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="9">
-        <v>24.280834485778101</v>
+      <c r="E15" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -14890,8 +14899,8 @@
       <c r="D16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="9">
-        <v>24.280834485778101</v>
+      <c r="E16" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -14922,8 +14931,8 @@
       <c r="D17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="9">
-        <v>24.280834485778101</v>
+      <c r="E17" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -14961,8 +14970,8 @@
       <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="9">
-        <v>24.280834485778101</v>
+      <c r="E18" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -15002,8 +15011,8 @@
       <c r="D19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="9">
-        <v>24.280834485778101</v>
+      <c r="E19" s="18">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -15042,8 +15051,8 @@
       <c r="D20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="9">
-        <v>63.535048440452002</v>
+      <c r="E20" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -15082,8 +15091,8 @@
       <c r="D21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="9">
-        <v>63.535048440452002</v>
+      <c r="E21" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -15106,7 +15115,7 @@
       </c>
       <c r="M21" s="13">
         <f>IF($L$20+$K$12*$L$20/K$4*(K5-K$4)&lt;$L21,$L$20+$K$12*$L$20/K$4*(K5-K$4),$L21)</f>
-        <v>218.72522005317757</v>
+        <v>174.92478288153185</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -15122,8 +15131,8 @@
       <c r="D22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="9">
-        <v>63.535048440452002</v>
+      <c r="E22" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -15146,7 +15155,7 @@
       </c>
       <c r="M22" s="13">
         <f t="shared" ref="M22:M23" si="1">IF($L$20+$K$12*$L$20/K$4*(K6-K$4)&lt;$L22,$L$20+$K$12*$L$20/K$4*(K6-K$4),$L22)</f>
-        <v>239.97339950243591</v>
+        <v>204.59498957328589</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
@@ -15162,8 +15171,8 @@
       <c r="D23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="9">
-        <v>63.535048440452002</v>
+      <c r="E23" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -15186,7 +15195,7 @@
       </c>
       <c r="M23" s="13">
         <f t="shared" si="1"/>
-        <v>243.24930849017187</v>
+        <v>241.91587243757215</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
@@ -15202,8 +15211,8 @@
       <c r="D24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="9">
-        <v>63.535048440452002</v>
+      <c r="E24" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -15242,8 +15251,8 @@
       <c r="D25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9">
-        <v>63.535048440452002</v>
+      <c r="E25" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -15282,8 +15291,8 @@
       <c r="D26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="9">
-        <v>63.535048440452002</v>
+      <c r="E26" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -15322,8 +15331,8 @@
       <c r="D27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="9">
-        <v>63.535048440452002</v>
+      <c r="E27" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -15342,8 +15351,8 @@
       <c r="D28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="9">
-        <v>63.535048440452002</v>
+      <c r="E28" s="18">
+        <v>15.0232392376651</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -15355,8 +15364,8 @@
         <v>2025</v>
       </c>
       <c r="M28" s="16">
-        <f>M21/L21-1</f>
-        <v>-7.3492855181425787E-2</v>
+        <f t="shared" ref="M28:M33" si="3">M21/L21-1</f>
+        <v>-0.25902892631140539</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.35">
@@ -15369,8 +15378,8 @@
       <c r="D29" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="9">
-        <v>62.293468341928197</v>
+      <c r="E29" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -15382,8 +15391,8 @@
         <v>2030</v>
       </c>
       <c r="M29" s="16">
-        <f>M22/L22-1</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-0.14742638143437603</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
@@ -15396,8 +15405,8 @@
       <c r="D30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="9">
-        <v>62.293468341928197</v>
+      <c r="E30" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -15409,8 +15418,8 @@
         <v>2035</v>
       </c>
       <c r="M30" s="16">
-        <f>M23/L23-1</f>
-        <v>-3.2903677023038425E-3</v>
+        <f t="shared" si="3"/>
+        <v>-8.7540977574002143E-3</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.35">
@@ -15423,8 +15432,8 @@
       <c r="D31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="9">
-        <v>62.293468341928303</v>
+      <c r="E31" s="18">
+        <v>34.711977233205502</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -15438,7 +15447,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="M31" s="16">
-        <f>M24/L24-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15452,8 +15461,8 @@
       <c r="D32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="9">
-        <v>62.293468341928197</v>
+      <c r="E32" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -15465,7 +15474,7 @@
         <v>2045</v>
       </c>
       <c r="M32" s="16">
-        <f>M25/L25-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15479,8 +15488,8 @@
       <c r="D33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="9">
-        <v>62.293468341928197</v>
+      <c r="E33" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -15492,7 +15501,7 @@
         <v>2050</v>
       </c>
       <c r="M33" s="16">
-        <f>M26/L26-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15506,8 +15515,8 @@
       <c r="D34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9">
-        <v>62.293468341928303</v>
+      <c r="E34" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -15527,8 +15536,8 @@
       <c r="D35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="9">
-        <v>62.293468341928303</v>
+      <c r="E35" s="18">
+        <v>34.711977233205502</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -15548,8 +15557,8 @@
       <c r="D36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="9">
-        <v>62.293468341928303</v>
+      <c r="E36" s="18">
+        <v>34.711977233204898</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -15569,8 +15578,8 @@
       <c r="D37" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="9">
-        <v>62.293468341928197</v>
+      <c r="E37" s="18">
+        <v>34.711977233205502</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -15590,8 +15599,8 @@
       <c r="D38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="9">
-        <v>18.211540691266102</v>
+      <c r="E38" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -15611,8 +15620,8 @@
       <c r="D39" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="9">
-        <v>18.211540691266102</v>
+      <c r="E39" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -15632,8 +15641,8 @@
       <c r="D40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="9">
-        <v>18.211540691266102</v>
+      <c r="E40" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -15653,8 +15662,8 @@
       <c r="D41" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="9">
-        <v>18.211540691266102</v>
+      <c r="E41" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -15674,8 +15683,8 @@
       <c r="D42" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="9">
-        <v>18.211540691266102</v>
+      <c r="E42" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -15695,8 +15704,8 @@
       <c r="D43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="9">
-        <v>18.211540691266102</v>
+      <c r="E43" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -15716,8 +15725,8 @@
       <c r="D44" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="9">
-        <v>18.211540691266102</v>
+      <c r="E44" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -15737,8 +15746,8 @@
       <c r="D45" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="9">
-        <v>18.211540691266102</v>
+      <c r="E45" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -15758,8 +15767,8 @@
       <c r="D46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="9">
-        <v>18.211540691266102</v>
+      <c r="E46" s="18">
+        <v>21.1760512654979</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -15780,8 +15789,8 @@
       <c r="D47" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="9">
-        <v>14.977247037745601</v>
+      <c r="E47" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -15802,8 +15811,8 @@
       <c r="D48" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="9">
-        <v>14.977247037745601</v>
+      <c r="E48" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -15824,8 +15833,8 @@
       <c r="D49" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="9">
-        <v>14.977247037745601</v>
+      <c r="E49" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
@@ -15846,8 +15855,8 @@
       <c r="D50" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="9">
-        <v>14.977247037745601</v>
+      <c r="E50" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
@@ -15868,8 +15877,8 @@
       <c r="D51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="9">
-        <v>14.977247037745601</v>
+      <c r="E51" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -15890,8 +15899,8 @@
       <c r="D52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="9">
-        <v>14.977247037745601</v>
+      <c r="E52" s="18">
+        <v>4.1497894416869299</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -15912,8 +15921,8 @@
       <c r="D53" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="9">
-        <v>14.977247037745601</v>
+      <c r="E53" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -15934,8 +15943,8 @@
       <c r="D54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="9">
-        <v>14.977247037745601</v>
+      <c r="E54" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -15956,8 +15965,8 @@
       <c r="D55" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="9">
-        <v>14.977247037745601</v>
+      <c r="E55" s="18">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -15978,8 +15987,8 @@
       <c r="D56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E56" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -16000,8 +16009,8 @@
       <c r="D57" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E57" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -16022,8 +16031,8 @@
       <c r="D58" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E58" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -16044,8 +16053,8 @@
       <c r="D59" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E59" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -16066,8 +16075,8 @@
       <c r="D60" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E60" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -16088,8 +16097,8 @@
       <c r="D61" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E61" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -16110,8 +16119,8 @@
       <c r="D62" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E62" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
@@ -16132,8 +16141,8 @@
       <c r="D63" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E63" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
@@ -16153,8 +16162,8 @@
       <c r="D64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E64" s="18">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
@@ -16174,8 +16183,8 @@
       <c r="D65" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E65" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
@@ -16195,8 +16204,8 @@
       <c r="D66" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E66" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -16216,8 +16225,8 @@
       <c r="D67" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E67" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
@@ -16237,8 +16246,8 @@
       <c r="D68" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E68" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
@@ -16258,8 +16267,8 @@
       <c r="D69" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E69" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
@@ -16279,8 +16288,8 @@
       <c r="D70" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E70" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E70" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -16300,8 +16309,8 @@
       <c r="D71" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E71" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
@@ -16321,8 +16330,8 @@
       <c r="D72" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E72" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -16342,8 +16351,8 @@
       <c r="D73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E73" s="18">
+        <v>-122.652753393711</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -16363,8 +16372,8 @@
       <c r="D74" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E74" s="18">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
@@ -16384,8 +16393,8 @@
       <c r="D75" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E75" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E75" s="18">
+        <v>-56.503754088162601</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
@@ -16405,8 +16414,8 @@
       <c r="D76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E76" s="18">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
@@ -16426,8 +16435,8 @@
       <c r="D77" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E77" s="18">
+        <v>-64.375129649066494</v>
       </c>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -16447,8 +16456,8 @@
       <c r="D78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E78" s="18">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -16468,8 +16477,8 @@
       <c r="D79" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E79" s="18">
+        <v>-57.3946104489983</v>
       </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -16489,8 +16498,8 @@
       <c r="D80" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E80" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E80" s="18">
+        <v>-66.462617756164704</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
@@ -16510,8 +16519,8 @@
       <c r="D81" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E81" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E81" s="18">
+        <v>-65.583419989923399</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
@@ -16531,8 +16540,8 @@
       <c r="D82" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E82" s="18">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
@@ -16558,8 +16567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B346FBC2-DB60-4620-89E4-836C469AA046}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="G13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M28" sqref="I28:M33"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16613,8 +16622,8 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E2" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -16625,7 +16634,7 @@
       </c>
       <c r="K2" s="13">
         <f>E2</f>
-        <v>-2.2457682046742198</v>
+        <v>9.0316922644172806</v>
       </c>
       <c r="L2" s="13">
         <f>F2</f>
@@ -16648,8 +16657,8 @@
       <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E3" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -16660,7 +16669,7 @@
       </c>
       <c r="K3" s="13">
         <f>E11</f>
-        <v>24.280834485778101</v>
+        <v>8.9898262698002593</v>
       </c>
       <c r="L3" s="13">
         <f>F11</f>
@@ -16684,8 +16693,8 @@
       <c r="D4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E4" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -16696,7 +16705,7 @@
       </c>
       <c r="K4" s="13">
         <f>E20</f>
-        <v>63.535048440452002</v>
+        <v>15.0232392376651</v>
       </c>
       <c r="L4" s="13">
         <f>F20</f>
@@ -16719,8 +16728,8 @@
       <c r="D5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E5" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -16731,7 +16740,7 @@
       </c>
       <c r="K5" s="13">
         <f>E29</f>
-        <v>62.293468341928197</v>
+        <v>34.711977233204898</v>
       </c>
       <c r="L5" s="13">
         <f>F29</f>
@@ -16754,8 +16763,8 @@
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E6" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -16766,7 +16775,7 @@
       </c>
       <c r="K6" s="13">
         <f>E38</f>
-        <v>18.211540691266102</v>
+        <v>21.1760512654979</v>
       </c>
       <c r="L6" s="13">
         <f>F38</f>
@@ -16789,8 +16798,8 @@
       <c r="D7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E7" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -16801,7 +16810,7 @@
       </c>
       <c r="K7" s="13">
         <f>E47</f>
-        <v>14.977247037745601</v>
+        <v>4.1497894416852104</v>
       </c>
       <c r="L7" s="13">
         <f>F47</f>
@@ -16824,8 +16833,8 @@
       <c r="D8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E8" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -16836,7 +16845,7 @@
       </c>
       <c r="K8" s="13">
         <f>E56</f>
-        <v>-1.2088787852442899</v>
+        <v>-5.1040443793511603</v>
       </c>
       <c r="L8" s="13">
         <f>F56</f>
@@ -16859,8 +16868,8 @@
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E9" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -16871,7 +16880,7 @@
       </c>
       <c r="K9" s="13">
         <f>E66</f>
-        <v>-4.4651798005117804</v>
+        <v>-122.652753393711</v>
       </c>
       <c r="L9" s="13">
         <f>F66</f>
@@ -16894,8 +16903,8 @@
       <c r="D10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
-        <v>-2.2457682046742198</v>
+      <c r="E10" s="19">
+        <v>9.0316922644172806</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -16906,7 +16915,7 @@
       </c>
       <c r="K10" s="13">
         <f>E74</f>
-        <v>-6.3714064045683703</v>
+        <v>-66.369555750769905</v>
       </c>
       <c r="L10" s="13">
         <f>F74</f>
@@ -16929,8 +16938,8 @@
       <c r="D11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="9">
-        <v>24.280834485778101</v>
+      <c r="E11" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -16948,8 +16957,8 @@
       <c r="D12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="9">
-        <v>24.280834485778101</v>
+      <c r="E12" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -16972,8 +16981,8 @@
       <c r="D13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="9">
-        <v>24.280834485778101</v>
+      <c r="E13" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -16996,8 +17005,8 @@
       <c r="D14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="9">
-        <v>24.280834485778101</v>
+      <c r="E14" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -17014,8 +17023,8 @@
       <c r="D15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="9">
-        <v>24.280834485778101</v>
+      <c r="E15" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -17038,8 +17047,8 @@
       <c r="D16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="9">
-        <v>24.280834485778101</v>
+      <c r="E16" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -17067,8 +17076,8 @@
       <c r="D17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="9">
-        <v>24.280834485778101</v>
+      <c r="E17" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -17100,8 +17109,8 @@
       <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="9">
-        <v>24.280834485778101</v>
+      <c r="E18" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -17138,8 +17147,8 @@
       <c r="D19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="9">
-        <v>24.280834485778101</v>
+      <c r="E19" s="19">
+        <v>8.9898262698002593</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -17175,8 +17184,8 @@
       <c r="D20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="9">
-        <v>63.535048440452002</v>
+      <c r="E20" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -17212,8 +17221,8 @@
       <c r="D21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="9">
-        <v>63.535048440452002</v>
+      <c r="E21" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -17233,7 +17242,7 @@
       </c>
       <c r="M21" s="13">
         <f>IF($L$20+$K$12*$L$20/K$4*(K5-K$4)&lt;$L21,$L$20+$K$12*$L$20/K$4*(K5-K$4),$L21)</f>
-        <v>522.64090880675337</v>
+        <v>435.95747368147954</v>
       </c>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -17249,8 +17258,8 @@
       <c r="D22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="9">
-        <v>63.535048440452002</v>
+      <c r="E22" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -17270,7 +17279,7 @@
       </c>
       <c r="M22" s="13">
         <f t="shared" ref="M22:M23" si="1">IF($L$20+$K$12*$L$20/K$4*(K6-K$4)&lt;$L22,$L$20+$K$12*$L$20/K$4*(K6-K$4),$L22)</f>
-        <v>564.93223294325207</v>
+        <v>494.67641812578427</v>
       </c>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
@@ -17286,8 +17295,8 @@
       <c r="D23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="9">
-        <v>63.535048440452002</v>
+      <c r="E23" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -17307,7 +17316,7 @@
       </c>
       <c r="M23" s="13">
         <f t="shared" si="1"/>
-        <v>571.17540677771956</v>
+        <v>568.53646467980707</v>
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
@@ -17323,8 +17332,8 @@
       <c r="D24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="9">
-        <v>63.535048440452002</v>
+      <c r="E24" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -17360,8 +17369,8 @@
       <c r="D25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9">
-        <v>63.535048440452002</v>
+      <c r="E25" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -17397,8 +17406,8 @@
       <c r="D26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="9">
-        <v>63.535048440452002</v>
+      <c r="E26" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -17434,8 +17443,8 @@
       <c r="D27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="9">
-        <v>63.535048440452002</v>
+      <c r="E27" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -17451,8 +17460,8 @@
       <c r="D28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="9">
-        <v>63.535048440452002</v>
+      <c r="E28" s="19">
+        <v>15.0232392376651</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -17461,8 +17470,8 @@
         <v>2025</v>
       </c>
       <c r="M28" s="16">
-        <f>M21/L21-1</f>
-        <v>-6.1503256410485263E-2</v>
+        <f t="shared" ref="M28:M33" si="3">M21/L21-1</f>
+        <v>-0.21715911919772535</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.35">
@@ -17475,8 +17484,8 @@
       <c r="D29" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="9">
-        <v>62.293468341928197</v>
+      <c r="E29" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -17485,8 +17494,8 @@
         <v>2030</v>
       </c>
       <c r="M29" s="16">
-        <f>M22/L22-1</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-0.12436149102599547</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
@@ -17499,8 +17508,8 @@
       <c r="D30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="9">
-        <v>62.293468341928197</v>
+      <c r="E30" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -17509,8 +17518,8 @@
         <v>2035</v>
       </c>
       <c r="M30" s="16">
-        <f>M23/L23-1</f>
-        <v>-4.726540188075834E-3</v>
+        <f t="shared" si="3"/>
+        <v>-9.3248982421276772E-3</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.35">
@@ -17523,8 +17532,8 @@
       <c r="D31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="9">
-        <v>62.293468341928303</v>
+      <c r="E31" s="19">
+        <v>34.711977233205502</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -17535,7 +17544,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="M31" s="16">
-        <f>M24/L24-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -17549,8 +17558,8 @@
       <c r="D32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="9">
-        <v>62.293468341928197</v>
+      <c r="E32" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -17559,7 +17568,7 @@
         <v>2045</v>
       </c>
       <c r="M32" s="16">
-        <f>M25/L25-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -17573,8 +17582,8 @@
       <c r="D33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="9">
-        <v>62.293468341928197</v>
+      <c r="E33" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -17583,7 +17592,7 @@
         <v>2050</v>
       </c>
       <c r="M33" s="16">
-        <f>M26/L26-1</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -17597,8 +17606,8 @@
       <c r="D34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9">
-        <v>62.293468341928303</v>
+      <c r="E34" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -17615,8 +17624,8 @@
       <c r="D35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="9">
-        <v>62.293468341928303</v>
+      <c r="E35" s="19">
+        <v>34.711977233205502</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -17633,8 +17642,8 @@
       <c r="D36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="9">
-        <v>62.293468341928303</v>
+      <c r="E36" s="19">
+        <v>34.711977233204898</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -17651,8 +17660,8 @@
       <c r="D37" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="9">
-        <v>62.293468341928197</v>
+      <c r="E37" s="19">
+        <v>34.711977233205502</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -17669,8 +17678,8 @@
       <c r="D38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="9">
-        <v>18.211540691266102</v>
+      <c r="E38" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -17687,8 +17696,8 @@
       <c r="D39" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="9">
-        <v>18.211540691266102</v>
+      <c r="E39" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -17705,8 +17714,8 @@
       <c r="D40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="9">
-        <v>18.211540691266102</v>
+      <c r="E40" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -17723,8 +17732,8 @@
       <c r="D41" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="9">
-        <v>18.211540691266102</v>
+      <c r="E41" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -17741,8 +17750,8 @@
       <c r="D42" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="9">
-        <v>18.211540691266102</v>
+      <c r="E42" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -17759,8 +17768,8 @@
       <c r="D43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="9">
-        <v>18.211540691266102</v>
+      <c r="E43" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -17777,8 +17786,8 @@
       <c r="D44" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="9">
-        <v>18.211540691266102</v>
+      <c r="E44" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -17795,8 +17804,8 @@
       <c r="D45" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="9">
-        <v>18.211540691266102</v>
+      <c r="E45" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -17813,8 +17822,8 @@
       <c r="D46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="9">
-        <v>18.211540691266102</v>
+      <c r="E46" s="19">
+        <v>21.1760512654979</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -17832,8 +17841,8 @@
       <c r="D47" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="9">
-        <v>14.977247037745601</v>
+      <c r="E47" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -17851,8 +17860,8 @@
       <c r="D48" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="9">
-        <v>14.977247037745601</v>
+      <c r="E48" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -17870,8 +17879,8 @@
       <c r="D49" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="9">
-        <v>14.977247037745601</v>
+      <c r="E49" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
@@ -17889,8 +17898,8 @@
       <c r="D50" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="9">
-        <v>14.977247037745601</v>
+      <c r="E50" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
@@ -17908,8 +17917,8 @@
       <c r="D51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="9">
-        <v>14.977247037745601</v>
+      <c r="E51" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -17927,8 +17936,8 @@
       <c r="D52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="9">
-        <v>14.977247037745601</v>
+      <c r="E52" s="19">
+        <v>4.1497894416869299</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -17946,8 +17955,8 @@
       <c r="D53" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="9">
-        <v>14.977247037745601</v>
+      <c r="E53" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -17965,8 +17974,8 @@
       <c r="D54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="9">
-        <v>14.977247037745601</v>
+      <c r="E54" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -17984,8 +17993,8 @@
       <c r="D55" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="9">
-        <v>14.977247037745601</v>
+      <c r="E55" s="19">
+        <v>4.1497894416852104</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -18003,8 +18012,8 @@
       <c r="D56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E56" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -18022,8 +18031,8 @@
       <c r="D57" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E57" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -18041,8 +18050,8 @@
       <c r="D58" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E58" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -18060,8 +18069,8 @@
       <c r="D59" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E59" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -18079,8 +18088,8 @@
       <c r="D60" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E60" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -18098,8 +18107,8 @@
       <c r="D61" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E61" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -18117,8 +18126,8 @@
       <c r="D62" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E62" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
@@ -18136,8 +18145,8 @@
       <c r="D63" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E63" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
@@ -18154,8 +18163,8 @@
       <c r="D64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="9">
-        <v>-1.2088787852442899</v>
+      <c r="E64" s="19">
+        <v>-5.1040443793511603</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
@@ -18172,8 +18181,8 @@
       <c r="D65" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E65" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
@@ -18190,8 +18199,8 @@
       <c r="D66" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E66" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -18208,8 +18217,8 @@
       <c r="D67" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E67" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
@@ -18226,8 +18235,8 @@
       <c r="D68" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E68" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
@@ -18244,8 +18253,8 @@
       <c r="D69" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E69" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
@@ -18262,8 +18271,8 @@
       <c r="D70" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E70" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E70" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -18280,8 +18289,8 @@
       <c r="D71" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E71" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
@@ -18298,8 +18307,8 @@
       <c r="D72" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E72" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -18316,8 +18325,8 @@
       <c r="D73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="9">
-        <v>-4.4651798005117804</v>
+      <c r="E73" s="19">
+        <v>-122.652753393711</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -18334,8 +18343,8 @@
       <c r="D74" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E74" s="19">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
@@ -18352,8 +18361,8 @@
       <c r="D75" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E75" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E75" s="19">
+        <v>-56.503754088162601</v>
       </c>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
@@ -18370,8 +18379,8 @@
       <c r="D76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E76" s="19">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
@@ -18388,8 +18397,8 @@
       <c r="D77" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E77" s="19">
+        <v>-64.375129649066494</v>
       </c>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -18406,8 +18415,8 @@
       <c r="D78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E78" s="19">
+        <v>-66.369555750769905</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -18424,8 +18433,8 @@
       <c r="D79" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E79" s="19">
+        <v>-57.3946104489983</v>
       </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -18442,8 +18451,8 @@
       <c r="D80" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E80" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E80" s="19">
+        <v>-66.462617756164704</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
@@ -18460,8 +18469,8 @@
       <c r="D81" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E81" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E81" s="19">
+        <v>-65.583419989923399</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
@@ -18478,8 +18487,8 @@
       <c r="D82" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="9">
-        <v>-6.3714064045683703</v>
+      <c r="E82" s="19">
+        <v>-57.394610448998201</v>
       </c>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
@@ -18503,7 +18512,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="K20" sqref="K18:L20"/>
+      <selection activeCell="I21" sqref="A21:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>